<commit_message>
MTPO - Fixes to tiger training lua script, updates to tiger training speadsheet, some more vaues mapped in the MTPO RAM map
</commit_message>
<xml_diff>
--- a/MTPO/TigerTraining.xlsx
+++ b/MTPO/TigerTraining.xlsx
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -591,7 +591,7 @@
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -605,15 +605,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="13">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B2" s="21">
-        <v>115</v>
+        <v>194</v>
       </c>
       <c r="C2" s="15">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>0</v>
@@ -625,10 +625,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
+    <row r="3" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A3" s="13">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>41</v>
+      </c>
       <c r="F3" s="13">
         <v>354</v>
       </c>
@@ -638,32 +644,60 @@
       <c r="H3" s="15">
         <v>685</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="13"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="15"/>
+      <c r="J3">
+        <f>13+16+31</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="13">
+        <v>143</v>
+      </c>
+      <c r="B4" s="14">
+        <v>300</v>
+      </c>
+      <c r="C4" s="15">
+        <v>205</v>
+      </c>
+      <c r="F4" s="13">
+        <v>55</v>
+      </c>
+      <c r="G4" s="21">
+        <v>115</v>
+      </c>
+      <c r="H4" s="15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="13">
+        <v>81</v>
+      </c>
+      <c r="B5" s="21">
+        <v>150</v>
+      </c>
+      <c r="C5" s="15">
+        <v>91</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="13"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="15"/>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13">
+        <v>31</v>
+      </c>
+      <c r="B6" s="21">
+        <v>60</v>
+      </c>
+      <c r="C6" s="15">
+        <v>40</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="21"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="13"/>
       <c r="B7" s="21"/>
       <c r="C7" s="15"/>
@@ -671,7 +705,7 @@
       <c r="G7" s="21"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="13"/>
       <c r="B8" s="21"/>
       <c r="C8" s="15"/>
@@ -679,7 +713,7 @@
       <c r="G8" s="21"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="13"/>
       <c r="B9" s="21"/>
       <c r="C9" s="15"/>
@@ -687,7 +721,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="13"/>
       <c r="B10" s="21"/>
       <c r="C10" s="15"/>
@@ -695,7 +729,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="17"/>
@@ -703,38 +737,38 @@
       <c r="G11" s="21"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="18">
         <f>SUM(A2:A11)</f>
-        <v>55</v>
+        <v>372</v>
       </c>
       <c r="B12" s="19">
         <f>SUM(B2:B11)</f>
-        <v>115</v>
+        <v>754</v>
       </c>
       <c r="C12" s="20">
         <f>SUM(C2:C11)</f>
-        <v>83</v>
+        <v>514</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="9"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="F13" s="18">
         <f>SUM(F3:F12)</f>
-        <v>354</v>
+        <v>409</v>
       </c>
       <c r="G13" s="19">
         <f>SUM(G3:G12)</f>
-        <v>835</v>
+        <v>950</v>
       </c>
       <c r="H13" s="20">
         <f>SUM(H3:H12)</f>
-        <v>685</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,17 +778,17 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
       <c r="A15" s="3">
         <f>ROUND(A12/B12*100,1)</f>
-        <v>47.8</v>
+        <v>49.3</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7">
         <f>ROUND(C12/B12,2)</f>
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>6</v>
@@ -768,17 +802,17 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="F16" s="3">
         <f>ROUND(F13/G13*100,1)</f>
-        <v>42.4</v>
+        <v>43.1</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="7">
         <f>ROUND(H13/G13,2)</f>
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>6</v>
@@ -792,7 +826,7 @@
     <row r="18" spans="1:3">
       <c r="A18">
         <f>ROUND(((A15/100)*(A15/100)) * 100, 2)</f>
-        <v>22.85</v>
+        <v>24.3</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -804,7 +838,7 @@
     <row r="19" spans="1:3">
       <c r="A19">
         <f>ROUND(((A15/100)*(A15/100)*(A15/100)) * 100, 2)</f>
-        <v>10.92</v>
+        <v>11.98</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -816,7 +850,7 @@
     <row r="20" spans="1:3">
       <c r="A20">
         <f>ROUND(((A15/100)*(A15/100)*(A15/100) * (A15/100)) * 100, 2)</f>
-        <v>5.22</v>
+        <v>5.91</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>

</xml_diff>